<commit_message>
Co-authored-by: Barry Ng <barryyng@users.noreply.github.com> Co-authored-by: Frizzante16 <Frizzante16@users.noreply.github.com> Co-authored-by: dragon21356 <dragon21356@users.noreply.github.com> Co-authored-by: #MANI SENTHILNATHAN VIGNESH# <VIGNESH024@e.ntu.edu.sg>
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/suggestions.xlsx
+++ b/OOPproj2002/src/pkg_camp/suggestions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="8">
   <si>
     <t>Camp Name</t>
   </si>
@@ -26,13 +26,16 @@
     <t>Approval Status</t>
   </si>
   <si>
-    <t>chicken rice</t>
+    <t>testsuggestion</t>
   </si>
   <si>
     <t>YCHERN</t>
   </si>
   <si>
-    <t>testsuggestion</t>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -77,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,23 +122,9 @@
         <v>5</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="b" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D4" t="b" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>